<commit_message>
implemeted few changes in Assertions
</commit_message>
<xml_diff>
--- a/AutomaticResumeFilter/src/resources/ARF Signup.xlsx
+++ b/AutomaticResumeFilter/src/resources/ARF Signup.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yashmittal2\Desktop\Automatic-Resume-Filter-Automation\AutomaticResumeFilter\src\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ksaravanakumar\Documents\New folder\AutomaticResumeFilter\src\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A27C6B9A-B3E6-44F9-9415-E58482F81446}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{360C6513-EB57-462B-BC92-BA280301D65A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{E2DA63AA-E650-44EA-865C-7A408172C52D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E2DA63AA-E650-44EA-865C-7A408172C52D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -63,16 +63,16 @@
     <t>prem</t>
   </si>
   <si>
-    <t>shankar1217</t>
-  </si>
-  <si>
-    <t>prem1217</t>
-  </si>
-  <si>
-    <t>shankar61@gmail.com</t>
-  </si>
-  <si>
-    <t>prem15@gmail.com</t>
+    <t>prem23@gmail.com</t>
+  </si>
+  <si>
+    <t>shankar1222</t>
+  </si>
+  <si>
+    <t>prem1222</t>
+  </si>
+  <si>
+    <t>shankar72@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -438,15 +438,15 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="6" width="21.81640625" customWidth="1"/>
+    <col min="1" max="6" width="21.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -466,15 +466,15 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>7</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D2">
         <v>12345678</v>
@@ -483,15 +483,15 @@
         <v>12345678</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>8</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D3">
         <v>12345456</v>

</xml_diff>

<commit_message>
HR add recruitment page updated
</commit_message>
<xml_diff>
--- a/AutomaticResumeFilter/src/resources/ARF Signup.xlsx
+++ b/AutomaticResumeFilter/src/resources/ARF Signup.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ksaravanakumar\Documents\New folder\AutomaticResumeFilter\src\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{360C6513-EB57-462B-BC92-BA280301D65A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A4B35CD-2DBB-41A8-8D8A-9C41AC94610D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E2DA63AA-E650-44EA-865C-7A408172C52D}"/>
   </bookViews>
@@ -63,16 +63,16 @@
     <t>prem</t>
   </si>
   <si>
-    <t>prem23@gmail.com</t>
-  </si>
-  <si>
-    <t>shankar1222</t>
-  </si>
-  <si>
-    <t>prem1222</t>
-  </si>
-  <si>
-    <t>shankar72@gmail.com</t>
+    <t>prem1227</t>
+  </si>
+  <si>
+    <t>shankar1227</t>
+  </si>
+  <si>
+    <t>shankar77@gmail.com</t>
+  </si>
+  <si>
+    <t>prem28@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -438,7 +438,7 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -471,7 +471,7 @@
         <v>7</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C2" t="s">
         <v>10</v>
@@ -488,10 +488,10 @@
         <v>8</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s">
         <v>9</v>
-      </c>
-      <c r="C3" t="s">
-        <v>11</v>
       </c>
       <c r="D3">
         <v>12345456</v>

</xml_diff>

<commit_message>
All tests successfully merged.
</commit_message>
<xml_diff>
--- a/AutomaticResumeFilter/src/resources/ARF Signup.xlsx
+++ b/AutomaticResumeFilter/src/resources/ARF Signup.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ksaravanakumar\Documents\New folder\AutomaticResumeFilter\src\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yashmittal2\Desktop\Automatic-Resume-Filter-Automation\AutomaticResumeFilter\src\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A4B35CD-2DBB-41A8-8D8A-9C41AC94610D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE551C02-344D-4945-A002-D7524ED2BE89}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E2DA63AA-E650-44EA-865C-7A408172C52D}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{E2DA63AA-E650-44EA-865C-7A408172C52D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -63,16 +63,16 @@
     <t>prem</t>
   </si>
   <si>
-    <t>prem1227</t>
-  </si>
-  <si>
-    <t>shankar1227</t>
-  </si>
-  <si>
-    <t>shankar77@gmail.com</t>
-  </si>
-  <si>
-    <t>prem28@gmail.com</t>
+    <t>shankar1239</t>
+  </si>
+  <si>
+    <t>prem1239</t>
+  </si>
+  <si>
+    <t>shankar87@gmail.com</t>
+  </si>
+  <si>
+    <t>prem38@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -438,15 +438,15 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="6" width="21.77734375" customWidth="1"/>
+    <col min="1" max="6" width="21.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -466,7 +466,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -474,7 +474,7 @@
         <v>11</v>
       </c>
       <c r="C2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D2">
         <v>12345678</v>
@@ -483,7 +483,7 @@
         <v>12345678</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -491,7 +491,7 @@
         <v>12</v>
       </c>
       <c r="C3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D3">
         <v>12345456</v>

</xml_diff>